<commit_message>
wrote code to pull europe climate data
</commit_message>
<xml_diff>
--- a/RawMaterials/data/JournalArticlesAlinaHasLookedAtToDate.xlsx
+++ b/RawMaterials/data/JournalArticlesAlinaHasLookedAtToDate.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alina\Documents\git\localadaptclim\RawMaterials\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00381BA-799B-4CDC-8CDC-AE53D280B49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1EF90A-2ADE-443A-BAE7-8D56464043D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{A8763C87-DFF9-4A08-964B-F5B5ED8150ED}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="1" activeTab="1" xr2:uid="{A8763C87-DFF9-4A08-964B-F5B5ED8150ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="ForAlina'sReference" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="272">
   <si>
     <t>To document everything I looked at for LA project</t>
   </si>
@@ -260,9 +262,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Effects of provenance, years, and planting location on bud burst of Douglas-fir. </t>
-  </si>
-  <si>
-    <t>YES?? Reach out to XXXX</t>
   </si>
   <si>
     <t>EA FAGUSY Petkova et al 2017</t>
@@ -789,6 +788,105 @@
   </si>
   <si>
     <t>Journal articles Alina has looked at to date</t>
+  </si>
+  <si>
+    <t>NA POPUBA Soola...lly etal 2013</t>
+  </si>
+  <si>
+    <t>Soolanayakanahally RY, Guy RD, Silim SN, Song M.</t>
+  </si>
+  <si>
+    <t>Timing of photoperiodic competency causes phenological mismatch in balsam poplar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Populus balsamifera </t>
+  </si>
+  <si>
+    <t>rob</t>
+  </si>
+  <si>
+    <t>need to get the location of the provenances</t>
+  </si>
+  <si>
+    <t>Panchen et al. 2014</t>
+  </si>
+  <si>
+    <t>Zoe A. Panchen,Richard B. Primack,Birgit Nordt,Elizabeth R. Ellwood,Albert-Dieter Stevens,Susanne S. Renner,Charles G. Willis,Robert Fahey,Alan Whittemore,Yanjun Du,Charles C. Davis</t>
+  </si>
+  <si>
+    <t>Leaf out times of temperate woody plants are related to phylogeny, deciduousness, growth habit and wood anatomy</t>
+  </si>
+  <si>
+    <t>not a provenance study</t>
+  </si>
+  <si>
+    <t>NA POPUBA Soola...lly etal 2015</t>
+  </si>
+  <si>
+    <t>Soolanayakanahally, R. Y., Guy, R. D., Street, N. R., Robinson, K. M., Silim, S. N., Albrectsen, B. R., &amp; Jansson, S.</t>
+  </si>
+  <si>
+    <t>Comparative physiology of allopatric Populus species: geographic clines in photosynthesis, height growth, and carbon isotope discrimination in common gardens</t>
+  </si>
+  <si>
+    <t>hmmm looks like there is no bb doy</t>
+  </si>
+  <si>
+    <t>EA POPUTR Soola...lly etal 2015</t>
+  </si>
+  <si>
+    <t>Populus tremula</t>
+  </si>
+  <si>
+    <t>NA CORNNU Kier et al. 2011</t>
+  </si>
+  <si>
+    <t>Karolyn R. Keir, Jordan B. Bemmels and Sally N. Aitken</t>
+  </si>
+  <si>
+    <t>Low genetic diversity, moderate local adaptation, and phylogeographic insights in Cornus nuttallii (Cornaceae)</t>
+  </si>
+  <si>
+    <t>Cornus nuttallii </t>
+  </si>
+  <si>
+    <t>Sally</t>
+  </si>
+  <si>
+    <t>no doy</t>
+  </si>
+  <si>
+    <t>NA QUERGA Huebert 2009</t>
+  </si>
+  <si>
+    <t>Huebert, Colin A.</t>
+  </si>
+  <si>
+    <t>The ecological and conservation genetics of Garry oak (Quercus garryana Dougl. ex Hook))</t>
+  </si>
+  <si>
+    <t>Quercus garryana</t>
+  </si>
+  <si>
+    <t>NA BETUPA Hawkins &amp; Dhar 2012</t>
+  </si>
+  <si>
+    <t>Christopher D.B. Hawkins &amp; Amalesh Dhar</t>
+  </si>
+  <si>
+    <t>Spring bud phenology of 18 Betula papyrifera populations in British Columbia</t>
+  </si>
+  <si>
+    <t>1998/1999</t>
+  </si>
+  <si>
+    <t>Betula papyrifera</t>
+  </si>
+  <si>
+    <t>Phenotypical traits and variability of six European beech (Fagus sylvatica L.) provenances on a test site in Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Mirko Liesebach</t>
   </si>
 </sst>
 </file>
@@ -854,7 +952,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -900,6 +998,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -991,7 +1101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1070,6 +1180,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1386,7 +1498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE5B864-EFCC-4037-984E-4A9021278338}">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
@@ -1400,7 +1512,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
@@ -1443,7 +1555,7 @@
         <v>12</v>
       </c>
       <c r="N5" s="45" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O5" s="43"/>
       <c r="P5" s="43"/>
@@ -1925,34 +2037,34 @@
         <v>11</v>
       </c>
       <c r="B16" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="D16" s="20" t="s">
         <v>77</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>78</v>
       </c>
       <c r="E16" s="19">
         <v>2017</v>
       </c>
       <c r="F16" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="19" t="s">
         <v>79</v>
-      </c>
-      <c r="G16" s="19" t="s">
-        <v>80</v>
       </c>
       <c r="H16" s="19" t="s">
         <v>17</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J16" s="19" t="s">
         <v>19</v>
       </c>
       <c r="K16" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L16" s="19" t="s">
         <v>62</v>
@@ -1972,13 +2084,13 @@
         <v>12</v>
       </c>
       <c r="B17" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="D17" s="20" t="s">
         <v>89</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>90</v>
       </c>
       <c r="E17" s="19">
         <v>2021</v>
@@ -1999,7 +2111,7 @@
         <v>19</v>
       </c>
       <c r="K17" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L17" s="19" t="s">
         <v>62</v>
@@ -2019,19 +2131,19 @@
         <v>13</v>
       </c>
       <c r="B18" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="D18" s="20" t="s">
         <v>93</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>94</v>
       </c>
       <c r="E18" s="19">
         <v>1993</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G18" s="19" t="s">
         <v>16</v>
@@ -2046,10 +2158,10 @@
         <v>19</v>
       </c>
       <c r="K18" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="L18" s="19" t="s">
         <v>96</v>
-      </c>
-      <c r="L18" s="19" t="s">
-        <v>97</v>
       </c>
       <c r="M18" s="21" t="s">
         <v>22</v>
@@ -2066,13 +2178,13 @@
         <v>14</v>
       </c>
       <c r="B19" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="D19" s="26" t="s">
         <v>99</v>
-      </c>
-      <c r="D19" s="26" t="s">
-        <v>100</v>
       </c>
       <c r="E19" s="19">
         <v>2008</v>
@@ -2087,16 +2199,16 @@
         <v>17</v>
       </c>
       <c r="I19" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J19" s="19" t="s">
         <v>32</v>
       </c>
       <c r="K19" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L19" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M19" s="21" t="s">
         <v>22</v>
@@ -2113,13 +2225,13 @@
         <v>15</v>
       </c>
       <c r="B20" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="D20" s="26" t="s">
         <v>104</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>105</v>
       </c>
       <c r="E20" s="19">
         <v>1999</v>
@@ -2143,7 +2255,7 @@
         <v>71</v>
       </c>
       <c r="L20" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M20" s="21" t="s">
         <v>22</v>
@@ -2160,19 +2272,19 @@
         <v>16</v>
       </c>
       <c r="B21" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="D21" s="26" t="s">
         <v>107</v>
-      </c>
-      <c r="D21" s="26" t="s">
-        <v>108</v>
       </c>
       <c r="E21" s="19">
         <v>2011</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G21" s="19" t="s">
         <v>17</v>
@@ -2181,13 +2293,13 @@
         <v>17</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J21" s="19" t="s">
         <v>19</v>
       </c>
       <c r="K21" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L21" s="19" t="s">
         <v>62</v>
@@ -2207,19 +2319,19 @@
         <v>17</v>
       </c>
       <c r="B22" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="D22" s="20" t="s">
         <v>112</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>113</v>
       </c>
       <c r="E22" s="19">
         <v>2021</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G22" s="19" t="s">
         <v>16</v>
@@ -2234,7 +2346,7 @@
         <v>32</v>
       </c>
       <c r="K22" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L22" s="19" t="s">
         <v>62</v>
@@ -2254,13 +2366,13 @@
         <v>18</v>
       </c>
       <c r="B23" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="D23" s="20" t="s">
         <v>117</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>118</v>
       </c>
       <c r="E23" s="19">
         <v>2020</v>
@@ -2281,7 +2393,7 @@
         <v>32</v>
       </c>
       <c r="K23" s="25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L23" s="19" t="s">
         <v>62</v>
@@ -2301,19 +2413,19 @@
         <v>19</v>
       </c>
       <c r="B24" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="D24" s="24" t="s">
         <v>84</v>
-      </c>
-      <c r="D24" s="24" t="s">
-        <v>85</v>
       </c>
       <c r="E24" s="23">
         <v>2012</v>
       </c>
       <c r="F24" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G24" s="23" t="s">
         <v>17</v>
@@ -2322,22 +2434,22 @@
         <v>17</v>
       </c>
       <c r="I24" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J24" s="23" t="s">
         <v>19</v>
       </c>
       <c r="K24" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L24" s="23" t="s">
         <v>62</v>
       </c>
       <c r="M24" s="28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N24" s="23" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="O24" s="23"/>
       <c r="P24" s="19"/>
@@ -2371,10 +2483,10 @@
       <c r="K25" s="23"/>
       <c r="L25" s="23"/>
       <c r="M25" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="N25" s="23" t="s">
         <v>231</v>
-      </c>
-      <c r="N25" s="23" t="s">
-        <v>232</v>
       </c>
       <c r="O25" s="19"/>
       <c r="P25" s="19"/>
@@ -2387,13 +2499,13 @@
         <v>21</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E26" s="19">
         <v>2007</v>
@@ -2410,10 +2522,10 @@
         <v>62</v>
       </c>
       <c r="M26" s="28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N26" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="O26" s="19"/>
       <c r="P26" s="19"/>
@@ -2426,13 +2538,13 @@
         <v>22</v>
       </c>
       <c r="B27" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="D27" s="24" t="s">
         <v>121</v>
-      </c>
-      <c r="C27" s="23" t="s">
-        <v>235</v>
-      </c>
-      <c r="D27" s="24" t="s">
-        <v>122</v>
       </c>
       <c r="E27" s="23">
         <v>1996</v>
@@ -2450,7 +2562,7 @@
         <v>39</v>
       </c>
       <c r="N27" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O27" s="23"/>
       <c r="P27" s="23"/>
@@ -2463,13 +2575,13 @@
         <v>23</v>
       </c>
       <c r="B28" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="D28" s="24" t="s">
         <v>124</v>
-      </c>
-      <c r="C28" s="23" t="s">
-        <v>236</v>
-      </c>
-      <c r="D28" s="24" t="s">
-        <v>125</v>
       </c>
       <c r="E28" s="23">
         <v>2018</v>
@@ -2498,13 +2610,13 @@
         <v>24</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E29" s="23">
         <v>2019</v>
@@ -2522,7 +2634,7 @@
         <v>39</v>
       </c>
       <c r="N29" s="23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O29" s="23"/>
       <c r="P29" s="23"/>
@@ -2571,7 +2683,7 @@
         <v>39</v>
       </c>
       <c r="N30" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O30" s="23"/>
       <c r="P30" s="23"/>
@@ -2584,13 +2696,13 @@
         <v>26</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C31" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="D31" s="24" t="s">
         <v>188</v>
-      </c>
-      <c r="D31" s="24" t="s">
-        <v>189</v>
       </c>
       <c r="E31" s="23">
         <v>1995</v>
@@ -2610,7 +2722,7 @@
         <v>39</v>
       </c>
       <c r="N31" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O31" s="23"/>
       <c r="P31" s="23"/>
@@ -2623,13 +2735,13 @@
         <v>27</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E32" s="23">
         <v>2014</v>
@@ -2649,7 +2761,7 @@
         <v>39</v>
       </c>
       <c r="N32" s="23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="O32" s="23"/>
       <c r="P32" s="23"/>
@@ -2662,13 +2774,13 @@
         <v>28</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E33" s="23">
         <v>2013</v>
@@ -2688,7 +2800,7 @@
         <v>39</v>
       </c>
       <c r="N33" s="30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="O33" s="31"/>
       <c r="P33" s="31"/>
@@ -2701,13 +2813,13 @@
         <v>29</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E34" s="19">
         <v>2017</v>
@@ -2725,7 +2837,7 @@
         <v>39</v>
       </c>
       <c r="N34" s="34" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O34" s="32"/>
       <c r="P34" s="32"/>
@@ -2738,13 +2850,13 @@
         <v>30</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C35" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="D35" s="20" t="s">
         <v>182</v>
-      </c>
-      <c r="D35" s="20" t="s">
-        <v>183</v>
       </c>
       <c r="E35" s="19">
         <v>2006</v>
@@ -2764,7 +2876,7 @@
         <v>39</v>
       </c>
       <c r="N35" s="19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O35" s="19"/>
       <c r="P35" s="19"/>
@@ -2777,13 +2889,13 @@
         <v>31</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C36" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="D36" s="20" t="s">
         <v>180</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>181</v>
       </c>
       <c r="E36" s="19">
         <v>2014</v>
@@ -2803,7 +2915,7 @@
         <v>39</v>
       </c>
       <c r="N36" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O36" s="19"/>
       <c r="P36" s="19"/>
@@ -2816,13 +2928,13 @@
         <v>32</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E37" s="19">
         <v>2015</v>
@@ -2842,7 +2954,7 @@
         <v>39</v>
       </c>
       <c r="N37" s="35" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O37" s="19"/>
       <c r="P37" s="19"/>
@@ -2855,13 +2967,13 @@
         <v>33</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E38" s="19">
         <v>2004</v>
@@ -2881,7 +2993,7 @@
         <v>39</v>
       </c>
       <c r="N38" s="35" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O38" s="19"/>
       <c r="P38" s="19"/>
@@ -2894,13 +3006,13 @@
         <v>34</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D39" s="36" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E39" s="19">
         <v>2016</v>
@@ -2920,7 +3032,7 @@
         <v>39</v>
       </c>
       <c r="N39" s="35" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O39" s="19"/>
       <c r="P39" s="19"/>
@@ -2933,13 +3045,13 @@
         <v>35</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C40" s="23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E40" s="19">
         <v>2015</v>
@@ -2959,7 +3071,7 @@
         <v>39</v>
       </c>
       <c r="N40" s="35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O40" s="19"/>
       <c r="P40" s="19"/>
@@ -2972,13 +3084,13 @@
         <v>36</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E41" s="19">
         <v>2017</v>
@@ -2998,7 +3110,7 @@
         <v>39</v>
       </c>
       <c r="N41" s="35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O41" s="19"/>
       <c r="P41" s="19"/>
@@ -3011,13 +3123,13 @@
         <v>37</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E42" s="19">
         <v>2002</v>
@@ -3037,7 +3149,7 @@
         <v>39</v>
       </c>
       <c r="N42" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O42" s="19"/>
       <c r="P42" s="19"/>
@@ -3050,13 +3162,13 @@
         <v>38</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E43" s="19">
         <v>1983</v>
@@ -3068,13 +3180,13 @@
       <c r="J43" s="19"/>
       <c r="K43" s="19"/>
       <c r="L43" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M43" s="29" t="s">
         <v>39</v>
       </c>
       <c r="N43" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O43" s="19"/>
       <c r="P43" s="19"/>
@@ -3087,13 +3199,13 @@
         <v>39</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E44" s="19">
         <v>1997</v>
@@ -3105,13 +3217,13 @@
       <c r="J44" s="19"/>
       <c r="K44" s="19"/>
       <c r="L44" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M44" s="29" t="s">
         <v>39</v>
       </c>
       <c r="N44" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O44" s="19"/>
       <c r="P44" s="19"/>
@@ -3124,13 +3236,13 @@
         <v>40</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E45" s="19">
         <v>1997</v>
@@ -3142,13 +3254,13 @@
       <c r="J45" s="19"/>
       <c r="K45" s="19"/>
       <c r="L45" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M45" s="29" t="s">
         <v>39</v>
       </c>
       <c r="N45" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O45" s="19"/>
       <c r="P45" s="19"/>
@@ -3161,13 +3273,13 @@
         <v>41</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E46" s="19">
         <v>2011</v>
@@ -3179,13 +3291,13 @@
       <c r="J46" s="19"/>
       <c r="K46" s="19"/>
       <c r="L46" s="19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M46" s="29" t="s">
         <v>39</v>
       </c>
       <c r="N46" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O46" s="19"/>
       <c r="P46" s="19"/>
@@ -3198,13 +3310,13 @@
         <v>42</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C47" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="D47" s="20" t="s">
         <v>194</v>
-      </c>
-      <c r="D47" s="20" t="s">
-        <v>195</v>
       </c>
       <c r="E47" s="19">
         <v>2006</v>
@@ -3216,13 +3328,13 @@
       <c r="J47" s="19"/>
       <c r="K47" s="19"/>
       <c r="L47" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="M47" s="29" t="s">
         <v>39</v>
       </c>
       <c r="N47" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O47" s="19"/>
       <c r="P47" s="19"/>
@@ -3235,13 +3347,13 @@
         <v>43</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C48" s="35" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E48" s="19">
         <v>2009</v>
@@ -3255,13 +3367,13 @@
       <c r="J48" s="19"/>
       <c r="K48" s="19"/>
       <c r="L48" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M48" s="29" t="s">
         <v>39</v>
       </c>
       <c r="N48" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O48" s="19"/>
       <c r="P48" s="19"/>
@@ -3275,10 +3387,10 @@
       </c>
       <c r="B49" s="19"/>
       <c r="C49" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E49" s="19">
         <v>2009</v>
@@ -3298,7 +3410,7 @@
         <v>39</v>
       </c>
       <c r="N49" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O49" s="19"/>
       <c r="P49" s="19"/>
@@ -3312,10 +3424,10 @@
       </c>
       <c r="B50" s="19"/>
       <c r="C50" s="19" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E50" s="19">
         <v>2010</v>
@@ -3335,7 +3447,7 @@
         <v>39</v>
       </c>
       <c r="N50" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O50" s="19"/>
       <c r="P50" s="19"/>
@@ -3348,13 +3460,13 @@
         <v>46</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D51" s="20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E51" s="19">
         <v>2007</v>
@@ -3374,7 +3486,7 @@
         <v>39</v>
       </c>
       <c r="N51" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O51" s="19"/>
       <c r="P51" s="19"/>
@@ -3387,13 +3499,13 @@
         <v>47</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C52" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="D52" s="20" t="s">
         <v>222</v>
-      </c>
-      <c r="D52" s="20" t="s">
-        <v>223</v>
       </c>
       <c r="E52" s="19">
         <v>2020</v>
@@ -3413,7 +3525,7 @@
         <v>39</v>
       </c>
       <c r="N52" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O52" s="19"/>
       <c r="P52" s="19"/>
@@ -3426,13 +3538,13 @@
         <v>48</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D53" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E53" s="19">
         <v>2016</v>
@@ -3452,7 +3564,7 @@
         <v>39</v>
       </c>
       <c r="N53" s="19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="O53" s="19"/>
       <c r="P53" s="19"/>
@@ -3465,13 +3577,13 @@
         <v>49</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D54" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E54" s="19">
         <v>1999</v>
@@ -3491,7 +3603,7 @@
         <v>39</v>
       </c>
       <c r="N54" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O54" s="19"/>
       <c r="P54" s="19"/>
@@ -3504,13 +3616,13 @@
         <v>50</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E55" s="19">
         <v>2010</v>
@@ -3530,7 +3642,7 @@
         <v>39</v>
       </c>
       <c r="N55" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O55" s="19"/>
       <c r="P55" s="19"/>
@@ -3543,13 +3655,13 @@
         <v>51</v>
       </c>
       <c r="B56" s="37" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C56" s="37" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D56" s="38" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E56" s="37">
         <v>2019</v>
@@ -3567,7 +3679,7 @@
         <v>39</v>
       </c>
       <c r="N56" s="37" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O56" s="37"/>
       <c r="P56" s="37"/>
@@ -3582,10 +3694,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCFEDDF9-A7E3-4B1E-8FC5-46B8D81A82AE}">
-  <dimension ref="A1:R56"/>
+  <dimension ref="A1:R64"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="R11" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4081,7 +4193,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="4" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="57.9" x14ac:dyDescent="0.6">
@@ -4090,34 +4202,34 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="D17" s="8" t="s">
         <v>77</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>78</v>
       </c>
       <c r="E17">
         <v>2017</v>
       </c>
       <c r="F17" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" t="s">
         <v>79</v>
-      </c>
-      <c r="G17" t="s">
-        <v>80</v>
       </c>
       <c r="H17" t="s">
         <v>17</v>
       </c>
       <c r="I17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J17" t="s">
         <v>19</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L17" t="s">
         <v>62</v>
@@ -4132,19 +4244,19 @@
         <v>13</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="E18" s="3">
         <v>2012</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>17</v>
@@ -4153,19 +4265,19 @@
         <v>17</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>19</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L18" s="3" t="s">
         <v>62</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="43.5" x14ac:dyDescent="0.6">
@@ -4174,13 +4286,13 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="D19" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>90</v>
       </c>
       <c r="E19">
         <v>2021</v>
@@ -4201,7 +4313,7 @@
         <v>19</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L19" t="s">
         <v>62</v>
@@ -4216,19 +4328,19 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" t="s">
         <v>92</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" s="8" t="s">
         <v>93</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>94</v>
       </c>
       <c r="E20">
         <v>1993</v>
       </c>
       <c r="F20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G20" t="s">
         <v>16</v>
@@ -4243,10 +4355,10 @@
         <v>19</v>
       </c>
       <c r="K20" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="L20" t="s">
         <v>96</v>
-      </c>
-      <c r="L20" t="s">
-        <v>97</v>
       </c>
       <c r="M20" t="s">
         <v>22</v>
@@ -4258,13 +4370,13 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="11" t="s">
         <v>99</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>100</v>
       </c>
       <c r="E21">
         <v>2008</v>
@@ -4279,16 +4391,16 @@
         <v>17</v>
       </c>
       <c r="I21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J21" t="s">
         <v>32</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M21" t="s">
         <v>22</v>
@@ -4300,13 +4412,13 @@
         <v>17</v>
       </c>
       <c r="B22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22" t="s">
         <v>103</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" s="11" t="s">
         <v>104</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>105</v>
       </c>
       <c r="E22">
         <v>1999</v>
@@ -4330,7 +4442,7 @@
         <v>71</v>
       </c>
       <c r="L22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M22" t="s">
         <v>22</v>
@@ -4342,19 +4454,19 @@
         <v>18</v>
       </c>
       <c r="B23" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" t="s">
         <v>106</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" s="11" t="s">
         <v>107</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>108</v>
       </c>
       <c r="E23">
         <v>2011</v>
       </c>
       <c r="F23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G23" t="s">
         <v>17</v>
@@ -4363,13 +4475,13 @@
         <v>17</v>
       </c>
       <c r="I23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J23" t="s">
         <v>19</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L23" t="s">
         <v>62</v>
@@ -4384,19 +4496,19 @@
         <v>19</v>
       </c>
       <c r="B24" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" t="s">
         <v>111</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" s="8" t="s">
         <v>112</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>113</v>
       </c>
       <c r="E24">
         <v>2021</v>
       </c>
       <c r="F24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G24" t="s">
         <v>16</v>
@@ -4411,7 +4523,7 @@
         <v>32</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L24" t="s">
         <v>62</v>
@@ -4426,13 +4538,13 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" t="s">
         <v>116</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" s="8" t="s">
         <v>117</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>118</v>
       </c>
       <c r="E25">
         <v>2020</v>
@@ -4453,7 +4565,7 @@
         <v>32</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L25" t="s">
         <v>62</v>
@@ -4468,11 +4580,11 @@
         <v>21</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E26" s="12">
         <v>1996</v>
@@ -4488,7 +4600,7 @@
         <v>39</v>
       </c>
       <c r="N26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -4497,11 +4609,11 @@
         <v>22</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E27" s="12">
         <v>2018</v>
@@ -4523,11 +4635,11 @@
         <v>23</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E28" s="12">
         <v>2019</v>
@@ -4543,7 +4655,7 @@
         <v>39</v>
       </c>
       <c r="N28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -4588,18 +4700,18 @@
         <v>39</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C30" t="s">
+        <v>187</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>188</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>189</v>
       </c>
       <c r="E30">
         <v>1995</v>
@@ -4611,18 +4723,18 @@
         <v>39</v>
       </c>
       <c r="N30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C31" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E31">
         <v>2007</v>
@@ -4631,21 +4743,21 @@
         <v>62</v>
       </c>
       <c r="M31" t="s">
+        <v>129</v>
+      </c>
+      <c r="N31" t="s">
         <v>130</v>
-      </c>
-      <c r="N31" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E32" s="12">
         <v>2014</v>
@@ -4657,18 +4769,18 @@
         <v>39</v>
       </c>
       <c r="N32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="2:18" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C33" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E33">
         <v>2013</v>
@@ -4680,7 +4792,7 @@
         <v>39</v>
       </c>
       <c r="N33" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="O33" s="14"/>
       <c r="P33" s="14"/>
@@ -4689,13 +4801,13 @@
     </row>
     <row r="34" spans="2:18" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E34">
         <v>2017</v>
@@ -4707,7 +4819,7 @@
         <v>39</v>
       </c>
       <c r="N34" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O34" s="14"/>
       <c r="P34" s="14"/>
@@ -4716,13 +4828,13 @@
     </row>
     <row r="35" spans="2:18" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C35" t="s">
+        <v>181</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>182</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>183</v>
       </c>
       <c r="E35">
         <v>2006</v>
@@ -4734,18 +4846,18 @@
         <v>39</v>
       </c>
       <c r="N35" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="2:18" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B36" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C36" t="s">
+        <v>179</v>
+      </c>
+      <c r="D36" s="8" t="s">
         <v>180</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>181</v>
       </c>
       <c r="E36">
         <v>2014</v>
@@ -4757,18 +4869,18 @@
         <v>39</v>
       </c>
       <c r="N36" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" spans="2:18" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C37" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E37">
         <v>2015</v>
@@ -4780,18 +4892,18 @@
         <v>39</v>
       </c>
       <c r="N37" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="2:18" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E38">
         <v>2004</v>
@@ -4803,18 +4915,18 @@
         <v>39</v>
       </c>
       <c r="N38" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="2:18" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B39" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E39">
         <v>2016</v>
@@ -4826,15 +4938,15 @@
         <v>39</v>
       </c>
       <c r="N39" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="40" spans="2:18" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E40">
         <v>2015</v>
@@ -4846,18 +4958,18 @@
         <v>39</v>
       </c>
       <c r="N40" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="2:18" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C41" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E41">
         <v>2017</v>
@@ -4869,18 +4981,18 @@
         <v>39</v>
       </c>
       <c r="N41" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="2:18" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B42" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C42" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E42">
         <v>2002</v>
@@ -4892,18 +5004,18 @@
         <v>39</v>
       </c>
       <c r="N42" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="2:18" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B43" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C43" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E43">
         <v>2010</v>
@@ -4915,18 +5027,18 @@
         <v>39</v>
       </c>
       <c r="N43" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="2:18" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B44" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C44" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E44">
         <v>2009</v>
@@ -4938,156 +5050,156 @@
         <v>39</v>
       </c>
       <c r="N44" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="45" spans="2:18" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B45" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C45" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E45">
         <v>1983</v>
       </c>
       <c r="L45" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M45" s="2" t="s">
         <v>39</v>
       </c>
       <c r="N45" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="46" spans="2:18" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B46" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C46" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E46">
         <v>1997</v>
       </c>
       <c r="L46" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M46" t="s">
         <v>39</v>
       </c>
       <c r="N46" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="47" spans="2:18" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B47" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C47" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E47">
         <v>1997</v>
       </c>
       <c r="L47" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M47" t="s">
         <v>39</v>
       </c>
       <c r="N47" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="48" spans="2:18" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B48" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C48" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E48">
         <v>2011</v>
       </c>
       <c r="L48" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M48" t="s">
         <v>39</v>
       </c>
       <c r="N48" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="49" spans="2:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B49" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C49" t="s">
+        <v>193</v>
+      </c>
+      <c r="D49" s="8" t="s">
         <v>194</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>195</v>
       </c>
       <c r="E49">
         <v>2006</v>
       </c>
       <c r="L49" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="M49" t="s">
         <v>39</v>
       </c>
       <c r="N49" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="50" spans="2:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B50" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E50">
         <v>2009</v>
       </c>
       <c r="L50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M50" t="s">
         <v>39</v>
       </c>
       <c r="N50" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C51" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E51">
         <v>2007</v>
@@ -5099,18 +5211,18 @@
         <v>39</v>
       </c>
       <c r="N51" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="52" spans="2:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B52" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C52" t="s">
+        <v>221</v>
+      </c>
+      <c r="D52" s="8" t="s">
         <v>222</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>223</v>
       </c>
       <c r="E52">
         <v>2020</v>
@@ -5122,18 +5234,18 @@
         <v>39</v>
       </c>
       <c r="N52" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="53" spans="2:14" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B53" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C53" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E53">
         <v>2016</v>
@@ -5145,18 +5257,18 @@
         <v>39</v>
       </c>
       <c r="N53" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="54" spans="2:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B54" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C54" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E54">
         <v>1999</v>
@@ -5168,18 +5280,18 @@
         <v>39</v>
       </c>
       <c r="N54" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="55" spans="2:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B55" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C55" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E55">
         <v>2010</v>
@@ -5191,18 +5303,18 @@
         <v>39</v>
       </c>
       <c r="N55" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="56" spans="2:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B56" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C56" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E56">
         <v>2019</v>
@@ -5214,7 +5326,267 @@
         <v>39</v>
       </c>
       <c r="N56" t="s">
-        <v>228</v>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="57" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B57" s="46" t="s">
+        <v>239</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="E57" s="4">
+        <v>2013</v>
+      </c>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K57" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="L57" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="M57" s="4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="58" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B58" t="s">
+        <v>245</v>
+      </c>
+      <c r="C58" t="s">
+        <v>246</v>
+      </c>
+      <c r="D58" t="s">
+        <v>247</v>
+      </c>
+      <c r="E58">
+        <v>2014</v>
+      </c>
+      <c r="L58" t="s">
+        <v>243</v>
+      </c>
+      <c r="M58" t="s">
+        <v>39</v>
+      </c>
+      <c r="N58" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="59" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B59" s="46" t="s">
+        <v>249</v>
+      </c>
+      <c r="C59" t="s">
+        <v>250</v>
+      </c>
+      <c r="D59" t="s">
+        <v>251</v>
+      </c>
+      <c r="E59">
+        <v>2015</v>
+      </c>
+      <c r="F59">
+        <v>2007</v>
+      </c>
+      <c r="G59" t="s">
+        <v>16</v>
+      </c>
+      <c r="H59" t="s">
+        <v>16</v>
+      </c>
+      <c r="I59" t="s">
+        <v>26</v>
+      </c>
+      <c r="J59" t="s">
+        <v>19</v>
+      </c>
+      <c r="K59" t="s">
+        <v>242</v>
+      </c>
+      <c r="L59" t="s">
+        <v>243</v>
+      </c>
+      <c r="M59" t="s">
+        <v>39</v>
+      </c>
+      <c r="N59" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="60" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B60" s="46" t="s">
+        <v>253</v>
+      </c>
+      <c r="C60" t="s">
+        <v>250</v>
+      </c>
+      <c r="D60" t="s">
+        <v>251</v>
+      </c>
+      <c r="E60">
+        <v>2015</v>
+      </c>
+      <c r="G60" t="s">
+        <v>17</v>
+      </c>
+      <c r="H60" t="s">
+        <v>17</v>
+      </c>
+      <c r="J60" t="s">
+        <v>19</v>
+      </c>
+      <c r="K60" t="s">
+        <v>254</v>
+      </c>
+      <c r="L60" t="s">
+        <v>243</v>
+      </c>
+      <c r="M60" t="s">
+        <v>39</v>
+      </c>
+      <c r="N60" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="61" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B61" t="s">
+        <v>255</v>
+      </c>
+      <c r="C61" t="s">
+        <v>256</v>
+      </c>
+      <c r="D61" t="s">
+        <v>257</v>
+      </c>
+      <c r="E61">
+        <v>2011</v>
+      </c>
+      <c r="G61" t="s">
+        <v>16</v>
+      </c>
+      <c r="H61" t="s">
+        <v>16</v>
+      </c>
+      <c r="I61" t="s">
+        <v>26</v>
+      </c>
+      <c r="J61" t="s">
+        <v>19</v>
+      </c>
+      <c r="K61" t="s">
+        <v>258</v>
+      </c>
+      <c r="L61" t="s">
+        <v>259</v>
+      </c>
+      <c r="M61" t="s">
+        <v>39</v>
+      </c>
+      <c r="N61" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="62" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B62" t="s">
+        <v>261</v>
+      </c>
+      <c r="C62" t="s">
+        <v>262</v>
+      </c>
+      <c r="D62" t="s">
+        <v>263</v>
+      </c>
+      <c r="E62">
+        <v>2009</v>
+      </c>
+      <c r="G62" t="s">
+        <v>16</v>
+      </c>
+      <c r="H62" t="s">
+        <v>16</v>
+      </c>
+      <c r="I62" t="s">
+        <v>26</v>
+      </c>
+      <c r="J62" t="s">
+        <v>19</v>
+      </c>
+      <c r="K62" t="s">
+        <v>264</v>
+      </c>
+      <c r="L62" t="s">
+        <v>259</v>
+      </c>
+      <c r="M62" t="s">
+        <v>39</v>
+      </c>
+      <c r="N62" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="63" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B63" s="47" t="s">
+        <v>265</v>
+      </c>
+      <c r="C63" s="47" t="s">
+        <v>266</v>
+      </c>
+      <c r="D63" s="47" t="s">
+        <v>267</v>
+      </c>
+      <c r="E63" s="47">
+        <v>2012</v>
+      </c>
+      <c r="F63" s="47" t="s">
+        <v>268</v>
+      </c>
+      <c r="G63" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="H63" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="I63" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="J63" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="K63" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="L63" s="47" t="s">
+        <v>243</v>
+      </c>
+      <c r="M63" s="47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="C64" t="s">
+        <v>271</v>
+      </c>
+      <c r="D64" t="s">
+        <v>270</v>
+      </c>
+      <c r="E64">
+        <v>2012</v>
       </c>
     </row>
   </sheetData>
@@ -5222,4 +5594,500 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7DC13B0-FF14-4521-8E3B-0B7026A35034}">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20:D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1">
+        <v>49</v>
+      </c>
+      <c r="B1">
+        <v>15</v>
+      </c>
+      <c r="C1">
+        <f>A1+B1/60</f>
+        <v>49.25</v>
+      </c>
+      <c r="E1">
+        <v>117</v>
+      </c>
+      <c r="F1">
+        <v>10</v>
+      </c>
+      <c r="G1">
+        <f>E1+F1/60</f>
+        <v>117.16666666666667</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>49</v>
+      </c>
+      <c r="B2">
+        <v>38</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C22" si="0">A2+B2/60</f>
+        <v>49.633333333333333</v>
+      </c>
+      <c r="E2">
+        <v>116</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ref="G2:G22" si="1">E2+F2/60</f>
+        <v>116.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>50</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>50.06666666666667</v>
+      </c>
+      <c r="E3">
+        <v>117</v>
+      </c>
+      <c r="F3">
+        <v>23</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="1"/>
+        <v>117.38333333333334</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>51</v>
+      </c>
+      <c r="B4">
+        <v>22</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>51.366666666666667</v>
+      </c>
+      <c r="E4">
+        <v>118</v>
+      </c>
+      <c r="F4">
+        <v>18</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>118.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>34</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>50.56666666666667</v>
+      </c>
+      <c r="E5">
+        <v>118</v>
+      </c>
+      <c r="F5">
+        <v>50</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>118.83333333333333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <v>46</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>50.766666666666666</v>
+      </c>
+      <c r="E6">
+        <v>119</v>
+      </c>
+      <c r="F6">
+        <v>32</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>119.53333333333333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <v>49</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>50.81666666666667</v>
+      </c>
+      <c r="E7">
+        <v>119</v>
+      </c>
+      <c r="F7">
+        <v>45</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>119.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>52</v>
+      </c>
+      <c r="B8">
+        <v>31</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>52.516666666666666</v>
+      </c>
+      <c r="E8">
+        <v>122</v>
+      </c>
+      <c r="F8">
+        <v>24</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>122.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>52</v>
+      </c>
+      <c r="B9">
+        <v>31</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>52.516666666666666</v>
+      </c>
+      <c r="E9">
+        <v>121</v>
+      </c>
+      <c r="F9">
+        <v>31</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>121.51666666666667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>52</v>
+      </c>
+      <c r="B10">
+        <v>47</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>52.783333333333331</v>
+      </c>
+      <c r="E10">
+        <v>122</v>
+      </c>
+      <c r="F10">
+        <v>14</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>122.23333333333333</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>53</v>
+      </c>
+      <c r="B11">
+        <v>47</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>53.783333333333331</v>
+      </c>
+      <c r="E11">
+        <v>122</v>
+      </c>
+      <c r="F11">
+        <v>38</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>122.63333333333334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>53</v>
+      </c>
+      <c r="B12">
+        <v>55</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>53.916666666666664</v>
+      </c>
+      <c r="E12">
+        <v>122</v>
+      </c>
+      <c r="F12">
+        <v>22</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>122.36666666666666</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>54</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>54.1</v>
+      </c>
+      <c r="E13">
+        <v>122</v>
+      </c>
+      <c r="F13">
+        <v>21</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>122.35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>54</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>54.133333333333333</v>
+      </c>
+      <c r="E14">
+        <v>121</v>
+      </c>
+      <c r="F14">
+        <v>47</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>121.78333333333333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>54</v>
+      </c>
+      <c r="B15">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>54.5</v>
+      </c>
+      <c r="E15">
+        <v>128</v>
+      </c>
+      <c r="F15">
+        <v>34</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>128.56666666666666</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>54</v>
+      </c>
+      <c r="B16">
+        <v>42</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>54.7</v>
+      </c>
+      <c r="E16">
+        <v>128</v>
+      </c>
+      <c r="F16">
+        <v>16</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>128.26666666666668</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>55</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>55.133333333333333</v>
+      </c>
+      <c r="E17">
+        <v>127</v>
+      </c>
+      <c r="F17">
+        <v>43</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>127.71666666666667</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>55</v>
+      </c>
+      <c r="B18">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>55.18333333333333</v>
+      </c>
+      <c r="E18">
+        <v>127</v>
+      </c>
+      <c r="F18">
+        <v>47</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>127.78333333333333</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>48</v>
+      </c>
+      <c r="B20">
+        <v>29</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>48.483333333333334</v>
+      </c>
+      <c r="D20">
+        <v>123.4</v>
+      </c>
+      <c r="E20">
+        <v>123</v>
+      </c>
+      <c r="F20">
+        <v>24</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>123.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>50</v>
+      </c>
+      <c r="B21">
+        <v>47</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>50.783333333333331</v>
+      </c>
+      <c r="D21">
+        <v>119.4</v>
+      </c>
+      <c r="E21">
+        <v>119</v>
+      </c>
+      <c r="F21">
+        <v>24</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>119.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>53</v>
+      </c>
+      <c r="B22">
+        <v>45</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>53.75</v>
+      </c>
+      <c r="D22">
+        <v>122.71666666666667</v>
+      </c>
+      <c r="E22">
+        <v>122</v>
+      </c>
+      <c r="F22">
+        <v>43</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>122.71666666666667</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
gathered data for altitudinal studies
</commit_message>
<xml_diff>
--- a/RawMaterials/data/JournalArticlesAlinaHasLookedAtToDate.xlsx
+++ b/RawMaterials/data/JournalArticlesAlinaHasLookedAtToDate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alina\Documents\git\localadaptclim\RawMaterials\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B1E323-6563-49D8-88F2-FEA2ABD0C823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE451C4-BB9C-4C8F-BE2E-00AB658F4B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="1" activeTab="1" xr2:uid="{A8763C87-DFF9-4A08-964B-F5B5ED8150ED}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>